<commit_message>
added LED timout for stations to increase battery life
</commit_message>
<xml_diff>
--- a/hardware/Costs.xlsx
+++ b/hardware/Costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timol\Documents\PlatformIO\Projects\Lichtschranke-reko\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D79AFC9-0917-43E9-B2D6-2D0772A410A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5E20FB-25EE-4AF3-B9D8-791E87D882A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="510" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Times</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>display</t>
   </si>
@@ -57,16 +54,143 @@
   </si>
   <si>
     <t>Time display</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>ky-40</t>
+  </si>
+  <si>
+    <t>qty</t>
+  </si>
+  <si>
+    <t>const per part</t>
+  </si>
+  <si>
+    <t>https://de.aliexpress.com/item/1005005988110355.html?spm=a2g0o.order_list.order_list_main.5.5e805c5fS69Qxe&amp;gatewayAdapt=glo2deu</t>
+  </si>
+  <si>
+    <t>gopro mount</t>
+  </si>
+  <si>
+    <t>https://de.aliexpress.com/item/4000283144125.html?spm=a2g0o.order_list.order_list_main.11.5e805c5fS69Qxe&amp;gatewayAdapt=glo2deu</t>
+  </si>
+  <si>
+    <t>antenna</t>
+  </si>
+  <si>
+    <t>https://de.aliexpress.com/item/32972870968.html?spm=a2g0o.order_list.order_list_main.17.5e805c5fS69Qxe&amp;gatewayAdapt=glo2deu</t>
+  </si>
+  <si>
+    <t>https://de.aliexpress.com/item/1005001265647648.html?spm=a2g0o.order_list.order_list_main.23.5e805c5fS69Qxe&amp;gatewayAdapt=glo2deu</t>
+  </si>
+  <si>
+    <t>boost converter</t>
+  </si>
+  <si>
+    <t>https://de.aliexpress.com/item/1005001632861136.html?spm=a2g0o.order_list.order_list_main.29.5e805c5fS69Qxe&amp;gatewayAdapt=glo2deu</t>
+  </si>
+  <si>
+    <t>Heltec lora v3</t>
+  </si>
+  <si>
+    <t>gopro screw</t>
+  </si>
+  <si>
+    <t>Rocker switch</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/-/en/RUNCCI-YUN-Rocker-Switch-Illuminated-Colour/dp/B07ZTHKNNH/ref=sr_1_4?crid=1N0Y0WQG92TFZ&amp;keywords=rocker+switch+led&amp;qid=1707065213&amp;sprefix=rocker+switch+le%2Caps%2C89&amp;sr=8-4</t>
+  </si>
+  <si>
+    <t>https://de.aliexpress.com/item/1005004993408849.html?spm=a2g0o.order_list.order_list_main.35.5e805c5fZ0IaML&amp;gatewayAdapt=glo2deu</t>
+  </si>
+  <si>
+    <t>https://de.aliexpress.com/item/1005005653753534.html?spm=a2g0o.order_list.order_list_main.41.5e805c5fZ0IaML&amp;gatewayAdapt=glo2deu</t>
+  </si>
+  <si>
+    <t>samsung 18650</t>
+  </si>
+  <si>
+    <t>18650 holder</t>
+  </si>
+  <si>
+    <t>https://www.berrybase.de/batteriehalter-fuer-1x-18650-mit-printanschluss?number=43997</t>
+  </si>
+  <si>
+    <t>cable</t>
+  </si>
+  <si>
+    <t>buzzer</t>
+  </si>
+  <si>
+    <t>Stativ</t>
+  </si>
+  <si>
+    <t>sma connector</t>
+  </si>
+  <si>
+    <t>liion charger</t>
+  </si>
+  <si>
+    <t>https://www.berrybase.de/ladeplatine-fuer-3-7v-liion/lipo-akkus-mit-ausgang-usb-type-c-buchse-loetpads-1000ma</t>
+  </si>
+  <si>
+    <t>station</t>
+  </si>
+  <si>
+    <t>ir transmitter</t>
+  </si>
+  <si>
+    <t>d. price</t>
+  </si>
+  <si>
+    <t>s. price</t>
+  </si>
+  <si>
+    <t>ir price</t>
+  </si>
+  <si>
+    <t>3D filament 100g</t>
+  </si>
+  <si>
+    <t>ir transmitter and receiver</t>
+  </si>
+  <si>
+    <t>Times (h)</t>
+  </si>
+  <si>
+    <t>Total costs</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>Station</t>
+  </si>
+  <si>
+    <t>Retail price</t>
+  </si>
+  <si>
+    <t>Profit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,13 +198,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -92,15 +243,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -379,78 +538,819 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" customWidth="1"/>
+    <col min="11" max="11" width="23.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3">
+        <f>J2*I2</f>
+        <v>0.75</v>
+      </c>
+      <c r="L2" s="5">
+        <v>1</v>
+      </c>
+      <c r="M2" s="3">
+        <f>L2*I2</f>
+        <v>0.75</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3">
+        <f>N2*I2</f>
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <f>B3*D1</f>
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3">
+        <v>2.31</v>
+      </c>
+      <c r="H3">
         <v>5</v>
       </c>
-      <c r="D1">
+      <c r="I3" s="3">
+        <f t="shared" ref="I3:I18" si="0">G3/H3</f>
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3">
+        <f t="shared" ref="K3:K17" si="1">J3*I3</f>
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="L3" s="5">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3">
+        <f t="shared" ref="M3:M17" si="2">L3*I3</f>
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3" s="3">
+        <f t="shared" ref="O3:O17" si="3">N3*I3</f>
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="P3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3">
+        <v>12.2</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="0"/>
+        <v>1.5249999999999999</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="1"/>
+        <v>1.5249999999999999</v>
+      </c>
+      <c r="L4" s="5">
+        <v>1</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" si="2"/>
+        <v>1.5249999999999999</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>9.59</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="0"/>
+        <v>9.59</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="1"/>
+        <v>9.59</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5">
+        <f>B5+B4</f>
+        <v>3</v>
+      </c>
+      <c r="D6" s="2">
+        <f>B6*D1</f>
+        <v>60</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1.38</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.27599999999999997</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="1"/>
+        <v>0.27599999999999997</v>
+      </c>
+      <c r="L6" s="5">
+        <v>2</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" si="2"/>
+        <v>0.55199999999999994</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6" s="3">
+        <f t="shared" si="3"/>
+        <v>0.27599999999999997</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="G7" s="3">
+        <v>17.489999999999998</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="0"/>
+        <v>17.489999999999998</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="1"/>
+        <v>17.489999999999998</v>
+      </c>
+      <c r="L7" s="5">
+        <v>1</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="2"/>
+        <v>17.489999999999998</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2.73</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="1"/>
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="L8" s="5">
+        <v>1</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="2"/>
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8" s="3">
+        <f t="shared" si="3"/>
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="F9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="G9" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="J9">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
-        <v>3.125E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <f>B5+B4</f>
-        <v>0.11458333333333333</v>
-      </c>
-      <c r="D6" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1"/>
+      <c r="K9" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L9" s="5">
+        <v>1</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9" s="3">
+        <f t="shared" si="3"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="3">
+        <v>7.99</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.99875000000000003</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="1"/>
+        <v>0.99875000000000003</v>
+      </c>
+      <c r="L10" s="5">
+        <v>1</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" si="2"/>
+        <v>0.99875000000000003</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10" s="3">
+        <f t="shared" si="3"/>
+        <v>0.99875000000000003</v>
+      </c>
+      <c r="P10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="3">
+        <v>6.1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="0"/>
+        <v>6.1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="1"/>
+        <v>6.1</v>
+      </c>
+      <c r="L11" s="5">
+        <v>1</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" si="2"/>
+        <v>6.1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11" s="3">
+        <f t="shared" si="3"/>
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.95</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="L12" s="5">
+        <v>1</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="P12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="L13" s="5">
+        <v>1</v>
+      </c>
+      <c r="M13" s="3">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13" s="3">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L14" s="5">
+        <v>1</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="L15" s="5">
+        <v>1</v>
+      </c>
+      <c r="M15" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="3">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="L16" s="5">
+        <v>1</v>
+      </c>
+      <c r="M16" s="3">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17" s="3">
+        <f>J17*I17</f>
+        <v>1.4</v>
+      </c>
+      <c r="L17" s="5">
+        <v>0</v>
+      </c>
+      <c r="M17" s="3">
+        <f>L17*I17</f>
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17" s="3">
+        <f>N17*I17</f>
+        <v>1.4</v>
+      </c>
+      <c r="P17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="3">
+        <v>21.99</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="0"/>
+        <v>21.99</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18" s="3">
+        <f>J18*I18</f>
+        <v>0</v>
+      </c>
+      <c r="L18" s="5">
+        <v>1</v>
+      </c>
+      <c r="M18" s="3">
+        <f>L18*I18</f>
+        <v>21.99</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18" s="3">
+        <f>N18*I18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+      <c r="J22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K22" s="6">
+        <f>SUM(K2:K21)</f>
+        <v>49.004750000000008</v>
+      </c>
+      <c r="L22" t="s">
+        <v>38</v>
+      </c>
+      <c r="M22" s="6">
+        <f>SUM(M2:M21)</f>
+        <v>57.780749999999998</v>
+      </c>
+      <c r="N22" t="s">
+        <v>39</v>
+      </c>
+      <c r="O22" s="6">
+        <f>SUM(O2:O21)</f>
+        <v>14.149749999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="8">
+        <f>K22+D3</f>
+        <v>89.004750000000001</v>
+      </c>
+      <c r="C23" s="2">
+        <v>300</v>
+      </c>
+      <c r="D23" s="3">
+        <f>C23-B23</f>
+        <v>210.99525</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="8">
+        <f>D6+M22+O22</f>
+        <v>131.93049999999999</v>
+      </c>
+      <c r="C24" s="2">
+        <v>250</v>
+      </c>
+      <c r="D24" s="3">
+        <f>C24-B24</f>
+        <v>118.06950000000001</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="P4" r:id="rId1" xr:uid="{1FF6BC22-BD5F-4087-99BD-82F952656679}"/>
+    <hyperlink ref="P5" r:id="rId2" xr:uid="{D69DD30D-121D-4148-BAF4-02B0B6427978}"/>
+    <hyperlink ref="P6" r:id="rId3" xr:uid="{C635B401-CE8A-4C2F-8F4E-596C63C65611}"/>
+    <hyperlink ref="P7" r:id="rId4" xr:uid="{3D3D0BD8-A4A9-4BC3-9A58-2A943B7849D3}"/>
+    <hyperlink ref="P8" r:id="rId5" xr:uid="{F4F73DC1-51CE-41A1-9DD6-1F739C965E78}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>